<commit_message>
Added last videos of floor 4 and floor 3
Excel with coordinates updates.
note - all videos under subfolders of each floor.
</commit_message>
<xml_diff>
--- a/mis/Creator coordinates.xlsx
+++ b/mis/Creator coordinates.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="19320" windowHeight="7740"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="19320" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
-    <sheet name="גיליון2" sheetId="2" r:id="rId2"/>
-    <sheet name="גיליון3" sheetId="3" r:id="rId3"/>
+    <sheet name="קומה 4" sheetId="1" r:id="rId1"/>
+    <sheet name="קומה 3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="27">
   <si>
     <t>מאיפה</t>
   </si>
@@ -27,18 +26,9 @@
     <t>Y</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>KEY</t>
   </si>
   <si>
@@ -58,6 +48,54 @@
   </si>
   <si>
     <t>דן פלדמן וגם 412</t>
+  </si>
+  <si>
+    <t>שירותים</t>
+  </si>
+  <si>
+    <t>412ג</t>
+  </si>
+  <si>
+    <t>412א</t>
+  </si>
+  <si>
+    <t>אורן</t>
+  </si>
+  <si>
+    <t>אור מאיר</t>
+  </si>
+  <si>
+    <t>מדרגות</t>
+  </si>
+  <si>
+    <t>עליה לקומה 5</t>
+  </si>
+  <si>
+    <t>חדר פרטי מדמח</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>camera Y</t>
+  </si>
+  <si>
+    <t>לקומה 2</t>
+  </si>
+  <si>
+    <t>פינת שירותים</t>
+  </si>
+  <si>
+    <t>לובי</t>
+  </si>
+  <si>
+    <t>קומה 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לובי </t>
+  </si>
+  <si>
+    <t>כניסה ראשית</t>
   </si>
 </sst>
 </file>
@@ -128,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,6 +186,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,51 +488,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9" style="4"/>
-    <col min="7" max="7" width="2.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="9" style="4"/>
-    <col min="13" max="13" width="13.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="4"/>
+    <col min="4" max="4" width="17.25" style="4" customWidth="1"/>
+    <col min="5" max="10" width="9" style="4"/>
+    <col min="11" max="11" width="13.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +533,7 @@
         <v>417</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>1.5</v>
@@ -513,16 +545,10 @@
         <v>-0.5</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
         <v>-90</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -538,10 +564,8 @@
         <v>11</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,16 +585,10 @@
         <v>12.5</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -578,7 +596,7 @@
         <v>417</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -586,10 +604,8 @@
         <v>-0.5</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -597,10 +613,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +622,7 @@
         <v>417</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>1.5</v>
@@ -620,16 +634,10 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
         <v>-180</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -637,7 +645,7 @@
         <v>401</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1">
@@ -645,10 +653,8 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +662,7 @@
         <v>401</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
         <v>1.5</v>
@@ -670,14 +676,8 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -685,7 +685,7 @@
         <v>417</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -693,10 +693,8 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -704,10 +702,8 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +711,7 @@
         <v>401</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
         <v>1.5</v>
@@ -727,22 +723,16 @@
         <v>-1.5</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
         <v>-90</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -750,7 +740,7 @@
         <v>408</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -758,10 +748,8 @@
         <v>10</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +757,7 @@
         <v>408</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1">
         <v>1.5</v>
@@ -781,16 +769,10 @@
         <v>-12</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -798,7 +780,7 @@
         <v>401</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -806,10 +788,8 @@
         <v>-0.5</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -817,10 +797,8 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +806,7 @@
         <v>408</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1">
         <v>1.5</v>
@@ -842,14 +820,8 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -857,7 +829,7 @@
         <v>413</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
@@ -865,10 +837,8 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +846,7 @@
         <v>413</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1">
         <v>1.5</v>
@@ -888,16 +858,10 @@
         <v>11</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -905,7 +869,7 @@
         <v>408</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
@@ -913,19 +877,530 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>401</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-13</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <v>-3</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-13</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1">
+        <v>401</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="G27" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F29" s="1">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1">
+        <v>401</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>-4.5</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>-85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>418</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1">
+        <v>-4</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>-4.5</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-5.9</v>
+      </c>
+      <c r="G34" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -935,24 +1410,845 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>305</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>303</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>-13</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1">
+        <v>305</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
+        <v>303</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>-5</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>305</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>303</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>-13</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
+        <v>305</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-16</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
+        <v>303</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <v>-5</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>305</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-14</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>-11.1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-10</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>305</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>-12.5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>305</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-13.5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <v>-12.6</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-2.6</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>-12.6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-4.8</v>
+      </c>
+      <c r="G19" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>305</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
+        <v>-13.6</v>
+      </c>
+      <c r="F20" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-15.6</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
+        <v>-6.7</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-3.5</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>-175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1">
+        <v>-12.5</v>
+      </c>
+      <c r="F25" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E27" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <v>306</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1">
+        <v>-4.3</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-4.3</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>306</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E29" s="1">
+        <v>-4.7</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-5.8</v>
+      </c>
+      <c r="G29" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E32" s="1">
+        <v>-6</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1">
+        <v>-1.4</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F34" s="1">
+        <v>6</v>
+      </c>
+      <c r="G34" s="1">
+        <v>-130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F37" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="G37" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <v>305</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1">
+        <v>-2.9</v>
+      </c>
+      <c r="F38" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1">
+        <v>305</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E39" s="1">
+        <v>-5.3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="G39" s="1">
+        <v>-38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1">
+        <v>305</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E42" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F42" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G42" s="1">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="E44" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="G44" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1">
+        <v>305</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1">
+        <v>8</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>